<commit_message>
Revert "attempt to add TOC filtering - not working"
This reverts commit 2b22d60104c7c87788e78bebdf11efa7fa9c3ced.
</commit_message>
<xml_diff>
--- a/RME_Rail_Fares/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/RME_Rail_Fares/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\RME_Rail_Fares\2_Route_and_times_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -181,12 +181,6 @@
   </si>
   <si>
     <t>Route6 - All TOCS</t>
-  </si>
-  <si>
-    <t>TOC Filter</t>
-  </si>
-  <si>
-    <t>All TOCs</t>
   </si>
 </sst>
 </file>
@@ -506,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,85 +540,86 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s">
-        <v>53</v>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>34</v>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>44</v>
@@ -639,16 +634,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>44</v>
@@ -663,96 +658,72 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code refactored to produce correct results
Unnecessary dictionaries and lists removed.  Simplification of the URL generation process
</commit_message>
<xml_diff>
--- a/RME_Rail_Fares/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/RME_Rail_Fares/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\RME_Rail_Fares\2_Route_and_times_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="52">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -162,9 +162,6 @@
     <t>,</t>
   </si>
   <si>
-    <t>1627,1630,1703, 2330</t>
-  </si>
-  <si>
     <t>Route 1 - All TOCS</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Route6 - All TOCS</t>
+  </si>
+  <si>
+    <t>1627,1630,1703,2330</t>
   </si>
 </sst>
 </file>
@@ -216,10 +216,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +502,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,22 +519,22 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -589,12 +588,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -666,7 +665,7 @@
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -735,61 +734,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>